<commit_message>
appraisal officials docs archived.
</commit_message>
<xml_diff>
--- a/CMMI for Dev. 2.0 L-3 Benchmark Appraisal schedule.xlsx
+++ b/CMMI for Dev. 2.0 L-3 Benchmark Appraisal schedule.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="127">
   <si>
     <t xml:space="preserve">Date </t>
   </si>
@@ -328,33 +328,15 @@
     <t>PR, RDM, VV, GOV, II</t>
   </si>
   <si>
-    <t>10:00 AM- 10:30 AM</t>
-  </si>
-  <si>
     <t>Training (OT)</t>
   </si>
   <si>
     <t>12:15 PM to 1.00 PM</t>
   </si>
   <si>
-    <t>2:00 PM 02:45 PM</t>
-  </si>
-  <si>
-    <t>03:00 PM to 03:45 PM</t>
-  </si>
-  <si>
-    <t>03:45 PM to 07:00 PM</t>
-  </si>
-  <si>
     <t>10:00 AM -11:00 AM</t>
   </si>
   <si>
-    <t>11:15 AM -12:00 Noon</t>
-  </si>
-  <si>
-    <t>12:00 Noon to 01:00 PM</t>
-  </si>
-  <si>
     <t>5th Nov. 22</t>
   </si>
   <si>
@@ -364,15 +346,6 @@
     <t xml:space="preserve">04:00 PM to 05:00 PM </t>
   </si>
   <si>
-    <t>10:00 AM -1:00 PM</t>
-  </si>
-  <si>
-    <t>2:00 PM to 03:30 PM</t>
-  </si>
-  <si>
-    <t>03.30 PM to 07:00 PM</t>
-  </si>
-  <si>
     <t>RSK , GOV, II</t>
   </si>
   <si>
@@ -409,19 +382,31 @@
     <t>Syoji</t>
   </si>
   <si>
-    <t>FAR Group</t>
-  </si>
-  <si>
-    <t>FAR Group Interviews</t>
-  </si>
-  <si>
-    <t>Abhishek Gupta, Harish Nagar, Ashish Choudhary, Sandeep Jain, Bharat Kakra, Rakesh Pandey, Gajesh Sharma, Ravi Jindal, Vikash, Abhishek Kumar, Mahesh, Rohit, Adarsh, Mayur, Deepesh, Sobhag, Syoji, Chandrashekhar</t>
-  </si>
-  <si>
-    <t>All</t>
-  </si>
-  <si>
     <t>GIL R&amp;D Conference Room</t>
+  </si>
+  <si>
+    <t>2:30 PM to 03:00 PM</t>
+  </si>
+  <si>
+    <t>10:30 AM -12:30 PM</t>
+  </si>
+  <si>
+    <t>03:30 PM to 04.15 PM</t>
+  </si>
+  <si>
+    <t>04.15 PM to 07:00 PM</t>
+  </si>
+  <si>
+    <t>03:00 PM to 04:00 PM</t>
+  </si>
+  <si>
+    <t>4.15 PM to 4.45 PM</t>
+  </si>
+  <si>
+    <t>04:45 PM to 07:00 PM</t>
+  </si>
+  <si>
+    <t>11:00 Noon to 012:00 Noon</t>
   </si>
 </sst>
 </file>
@@ -1027,6 +1012,9 @@
     <xf numFmtId="0" fontId="5" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1077,9 +1065,6 @@
     </xf>
     <xf numFmtId="15" fontId="4" fillId="4" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1398,10 +1383,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K37"/>
+  <dimension ref="A1:K36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="D20" sqref="D20:K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1505,7 +1490,7 @@
       </c>
     </row>
     <row r="5" spans="1:11" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="59" t="s">
+      <c r="A5" s="60" t="s">
         <v>86</v>
       </c>
       <c r="B5" s="10" t="s">
@@ -1521,18 +1506,18 @@
       <c r="F5" s="11"/>
       <c r="G5" s="11"/>
       <c r="H5" s="11" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="I5" s="11" t="s">
         <v>18</v>
       </c>
       <c r="J5" s="12" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="K5" s="13"/>
     </row>
     <row r="6" spans="1:11" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="60"/>
+      <c r="A6" s="61"/>
       <c r="B6" s="14" t="s">
         <v>35</v>
       </c>
@@ -1550,7 +1535,7 @@
         <v>18</v>
       </c>
       <c r="J6" s="12" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="K6" s="15"/>
     </row>
@@ -1568,128 +1553,134 @@
       <c r="K7" s="18"/>
     </row>
     <row r="8" spans="1:11" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="61" t="s">
+      <c r="A8" s="62" t="s">
         <v>87</v>
       </c>
       <c r="B8" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="C8" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" s="22"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="21" t="s">
+        <v>111</v>
+      </c>
+      <c r="H8" s="21" t="s">
         <v>112</v>
       </c>
-      <c r="C8" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14" t="s">
+      <c r="I8" s="21" t="s">
         <v>18</v>
       </c>
       <c r="J8" s="12" t="s">
-        <v>131</v>
-      </c>
-      <c r="K8" s="15"/>
+        <v>118</v>
+      </c>
+      <c r="K8" s="26" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="9" spans="1:11" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="62"/>
+      <c r="A9" s="63"/>
       <c r="B9" s="21" t="s">
+        <v>119</v>
+      </c>
+      <c r="C9" s="30" t="s">
+        <v>100</v>
+      </c>
+      <c r="D9" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" s="22"/>
+      <c r="F9" s="50"/>
+      <c r="G9" s="44" t="s">
+        <v>108</v>
+      </c>
+      <c r="H9" s="44" t="s">
         <v>113</v>
       </c>
-      <c r="C9" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="E9" s="22"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="21" t="s">
-        <v>120</v>
-      </c>
-      <c r="H9" s="21" t="s">
+      <c r="I9" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="J9" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="K9" s="51" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="63"/>
+      <c r="B10" s="24" t="s">
         <v>121</v>
       </c>
-      <c r="I9" s="21" t="s">
+      <c r="C10" s="23" t="s">
+        <v>94</v>
+      </c>
+      <c r="D10" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" s="32"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="H10" s="20" t="s">
+        <v>115</v>
+      </c>
+      <c r="I10" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="J10" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="K10" s="31" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="63"/>
+      <c r="B11" s="27" t="s">
+        <v>122</v>
+      </c>
+      <c r="C11" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" s="28"/>
+      <c r="F11" s="27"/>
+      <c r="G11" s="27"/>
+      <c r="H11" s="27"/>
+      <c r="I11" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="J9" s="12" t="s">
-        <v>131</v>
-      </c>
-      <c r="K9" s="26" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="62"/>
-      <c r="B10" s="27" t="s">
-        <v>114</v>
-      </c>
-      <c r="C10" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="D10" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="E10" s="28"/>
-      <c r="F10" s="27"/>
-      <c r="G10" s="27"/>
-      <c r="H10" s="27"/>
-      <c r="I10" s="27" t="s">
-        <v>18</v>
-      </c>
-      <c r="J10" s="12" t="s">
-        <v>131</v>
-      </c>
-      <c r="K10" s="29"/>
-    </row>
-    <row r="11" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="56"/>
-      <c r="B11" s="57"/>
-      <c r="C11" s="57"/>
-      <c r="D11" s="57"/>
-      <c r="E11" s="57"/>
-      <c r="F11" s="57"/>
-      <c r="G11" s="57"/>
-      <c r="H11" s="57"/>
-      <c r="I11" s="57"/>
-      <c r="J11" s="57"/>
-      <c r="K11" s="58"/>
-    </row>
-    <row r="12" spans="1:11" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="63" t="s">
+      <c r="J11" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="K11" s="29"/>
+    </row>
+    <row r="12" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="57"/>
+      <c r="B12" s="58"/>
+      <c r="C12" s="58"/>
+      <c r="D12" s="58"/>
+      <c r="E12" s="58"/>
+      <c r="F12" s="58"/>
+      <c r="G12" s="58"/>
+      <c r="H12" s="58"/>
+      <c r="I12" s="58"/>
+      <c r="J12" s="58"/>
+      <c r="K12" s="59"/>
+    </row>
+    <row r="13" spans="1:11" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="64" t="s">
         <v>88</v>
       </c>
-      <c r="B12" s="44" t="s">
-        <v>100</v>
-      </c>
-      <c r="C12" s="30" t="s">
-        <v>101</v>
-      </c>
-      <c r="D12" s="30" t="s">
-        <v>30</v>
-      </c>
-      <c r="E12" s="22"/>
-      <c r="F12" s="50"/>
-      <c r="G12" s="44" t="s">
-        <v>117</v>
-      </c>
-      <c r="H12" s="44" t="s">
-        <v>122</v>
-      </c>
-      <c r="I12" s="44" t="s">
-        <v>24</v>
-      </c>
-      <c r="J12" s="12" t="s">
-        <v>131</v>
-      </c>
-      <c r="K12" s="51" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="63"/>
       <c r="B13" s="24" t="s">
         <v>70</v>
       </c>
@@ -1705,54 +1696,54 @@
         <v>23</v>
       </c>
       <c r="H13" s="20" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="I13" s="20" t="s">
         <v>24</v>
       </c>
       <c r="J13" s="12" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="K13" s="31" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="63"/>
+    <row r="14" spans="1:11" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="64"/>
       <c r="B14" s="24" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C14" s="23" t="s">
-        <v>94</v>
+        <v>107</v>
       </c>
       <c r="D14" s="23" t="s">
         <v>30</v>
       </c>
       <c r="E14" s="32"/>
-      <c r="F14" s="20"/>
+      <c r="F14" s="23"/>
       <c r="G14" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="H14" s="20" t="s">
-        <v>124</v>
-      </c>
-      <c r="I14" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="H14" s="23" t="s">
+        <v>116</v>
+      </c>
+      <c r="I14" s="24" t="s">
         <v>24</v>
       </c>
       <c r="J14" s="12" t="s">
-        <v>131</v>
-      </c>
-      <c r="K14" s="31" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="63"/>
+        <v>118</v>
+      </c>
+      <c r="K14" s="25" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="64"/>
       <c r="B15" s="24" t="s">
-        <v>103</v>
+        <v>123</v>
       </c>
       <c r="C15" s="23" t="s">
-        <v>116</v>
+        <v>95</v>
       </c>
       <c r="D15" s="23" t="s">
         <v>30</v>
@@ -1760,54 +1751,56 @@
       <c r="E15" s="32"/>
       <c r="F15" s="23"/>
       <c r="G15" s="23" t="s">
-        <v>118</v>
+        <v>23</v>
       </c>
       <c r="H15" s="23" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="I15" s="24" t="s">
         <v>24</v>
       </c>
       <c r="J15" s="12" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="K15" s="25" t="s">
-        <v>33</v>
+        <v>99</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="63"/>
-      <c r="B16" s="24" t="s">
-        <v>104</v>
-      </c>
-      <c r="C16" s="23" t="s">
-        <v>95</v>
+      <c r="A16" s="64"/>
+      <c r="B16" s="36" t="s">
+        <v>124</v>
+      </c>
+      <c r="C16" s="21" t="s">
+        <v>92</v>
       </c>
       <c r="D16" s="23" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="E16" s="32"/>
-      <c r="F16" s="23"/>
+      <c r="F16" s="23" t="s">
+        <v>21</v>
+      </c>
       <c r="G16" s="23" t="s">
         <v>23</v>
       </c>
       <c r="H16" s="23" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="I16" s="24" t="s">
         <v>24</v>
       </c>
       <c r="J16" s="12" t="s">
-        <v>131</v>
-      </c>
-      <c r="K16" s="25" t="s">
-        <v>99</v>
+        <v>118</v>
+      </c>
+      <c r="K16" s="48" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="60"/>
+      <c r="A17" s="61"/>
       <c r="B17" s="14" t="s">
-        <v>105</v>
+        <v>125</v>
       </c>
       <c r="C17" s="14" t="s">
         <v>37</v>
@@ -1823,29 +1816,29 @@
         <v>24</v>
       </c>
       <c r="J17" s="12" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="K17" s="34"/>
     </row>
     <row r="18" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="70"/>
-      <c r="B18" s="71"/>
-      <c r="C18" s="71"/>
-      <c r="D18" s="71"/>
-      <c r="E18" s="71"/>
-      <c r="F18" s="71"/>
-      <c r="G18" s="71"/>
-      <c r="H18" s="71"/>
-      <c r="I18" s="71"/>
-      <c r="J18" s="71"/>
-      <c r="K18" s="72"/>
+      <c r="A18" s="71"/>
+      <c r="B18" s="72"/>
+      <c r="C18" s="72"/>
+      <c r="D18" s="72"/>
+      <c r="E18" s="72"/>
+      <c r="F18" s="72"/>
+      <c r="G18" s="72"/>
+      <c r="H18" s="72"/>
+      <c r="I18" s="72"/>
+      <c r="J18" s="72"/>
+      <c r="K18" s="73"/>
     </row>
     <row r="19" spans="1:11" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="64" t="s">
+      <c r="A19" s="65" t="s">
         <v>89</v>
       </c>
       <c r="B19" s="44" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C19" s="44" t="s">
         <v>91</v>
@@ -1861,169 +1854,155 @@
         <v>22</v>
       </c>
       <c r="H19" s="52" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="I19" s="35" t="s">
         <v>18</v>
       </c>
       <c r="J19" s="12" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="K19" s="53" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="65"/>
-      <c r="B20" s="21" t="s">
-        <v>107</v>
-      </c>
-      <c r="C20" s="21" t="s">
-        <v>92</v>
+    <row r="20" spans="1:11" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="66"/>
+      <c r="B20" s="49" t="s">
+        <v>126</v>
+      </c>
+      <c r="C20" s="23" t="s">
+        <v>39</v>
       </c>
       <c r="D20" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="E20" s="32"/>
-      <c r="F20" s="23" t="s">
-        <v>21</v>
-      </c>
-      <c r="G20" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="H20" s="23" t="s">
-        <v>126</v>
-      </c>
+        <v>85</v>
+      </c>
+      <c r="E20" s="23"/>
+      <c r="F20" s="23"/>
+      <c r="G20" s="23"/>
+      <c r="H20" s="23"/>
       <c r="I20" s="24" t="s">
         <v>24</v>
       </c>
       <c r="J20" s="12" t="s">
-        <v>131</v>
-      </c>
-      <c r="K20" s="48" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" ht="225.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="65"/>
-      <c r="B21" s="49" t="s">
-        <v>108</v>
+        <v>118</v>
+      </c>
+      <c r="K20" s="48"/>
+    </row>
+    <row r="21" spans="1:11" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="66"/>
+      <c r="B21" s="24" t="s">
+        <v>71</v>
       </c>
       <c r="C21" s="23" t="s">
-        <v>127</v>
+        <v>39</v>
       </c>
       <c r="D21" s="23" t="s">
         <v>85</v>
       </c>
-      <c r="E21" s="32"/>
+      <c r="E21" s="23"/>
       <c r="F21" s="23"/>
-      <c r="G21" s="23" t="s">
-        <v>128</v>
-      </c>
-      <c r="H21" s="23" t="s">
-        <v>129</v>
-      </c>
+      <c r="G21" s="23"/>
+      <c r="H21" s="23"/>
       <c r="I21" s="24" t="s">
         <v>24</v>
       </c>
       <c r="J21" s="12" t="s">
-        <v>131</v>
-      </c>
-      <c r="K21" s="48" t="s">
-        <v>130</v>
-      </c>
+        <v>118</v>
+      </c>
+      <c r="K21" s="48"/>
     </row>
     <row r="22" spans="1:11" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="65"/>
-      <c r="B22" s="24" t="s">
-        <v>71</v>
-      </c>
-      <c r="C22" s="23" t="s">
-        <v>39</v>
-      </c>
-      <c r="D22" s="23" t="s">
+      <c r="A22" s="67"/>
+      <c r="B22" s="36" t="s">
+        <v>72</v>
+      </c>
+      <c r="C22" s="43" t="s">
+        <v>40</v>
+      </c>
+      <c r="D22" s="43" t="s">
         <v>85</v>
       </c>
-      <c r="E22" s="23"/>
-      <c r="F22" s="23"/>
-      <c r="G22" s="23"/>
-      <c r="H22" s="23"/>
-      <c r="I22" s="24" t="s">
+      <c r="E22" s="43"/>
+      <c r="F22" s="43"/>
+      <c r="G22" s="43"/>
+      <c r="H22" s="43"/>
+      <c r="I22" s="36" t="s">
         <v>24</v>
       </c>
       <c r="J22" s="12" t="s">
-        <v>131</v>
-      </c>
-      <c r="K22" s="48"/>
-    </row>
-    <row r="23" spans="1:11" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="66"/>
-      <c r="B23" s="36" t="s">
-        <v>72</v>
-      </c>
-      <c r="C23" s="43" t="s">
-        <v>40</v>
-      </c>
-      <c r="D23" s="43" t="s">
-        <v>85</v>
-      </c>
-      <c r="E23" s="43"/>
-      <c r="F23" s="43"/>
-      <c r="G23" s="43"/>
-      <c r="H23" s="43"/>
-      <c r="I23" s="36" t="s">
+        <v>118</v>
+      </c>
+      <c r="K22" s="54"/>
+    </row>
+    <row r="23" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="57"/>
+      <c r="B23" s="58"/>
+      <c r="C23" s="58"/>
+      <c r="D23" s="58"/>
+      <c r="E23" s="58"/>
+      <c r="F23" s="58"/>
+      <c r="G23" s="58"/>
+      <c r="H23" s="58"/>
+      <c r="I23" s="58"/>
+      <c r="J23" s="58"/>
+      <c r="K23" s="59"/>
+    </row>
+    <row r="24" spans="1:11" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="68" t="s">
+        <v>103</v>
+      </c>
+      <c r="B24" s="35" t="s">
+        <v>42</v>
+      </c>
+      <c r="C24" s="30" t="s">
+        <v>41</v>
+      </c>
+      <c r="D24" s="35" t="s">
+        <v>38</v>
+      </c>
+      <c r="E24" s="35"/>
+      <c r="F24" s="30"/>
+      <c r="G24" s="30"/>
+      <c r="H24" s="30"/>
+      <c r="I24" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="J23" s="12" t="s">
-        <v>131</v>
-      </c>
-      <c r="K23" s="54"/>
-    </row>
-    <row r="24" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="56"/>
-      <c r="B24" s="57"/>
-      <c r="C24" s="57"/>
-      <c r="D24" s="57"/>
-      <c r="E24" s="57"/>
-      <c r="F24" s="57"/>
-      <c r="G24" s="57"/>
-      <c r="H24" s="57"/>
-      <c r="I24" s="57"/>
-      <c r="J24" s="57"/>
-      <c r="K24" s="58"/>
+      <c r="J24" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="K24" s="53"/>
     </row>
     <row r="25" spans="1:11" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="67" t="s">
-        <v>109</v>
-      </c>
-      <c r="B25" s="35" t="s">
-        <v>42</v>
-      </c>
-      <c r="C25" s="30" t="s">
-        <v>41</v>
-      </c>
-      <c r="D25" s="35" t="s">
-        <v>38</v>
-      </c>
-      <c r="E25" s="35"/>
-      <c r="F25" s="30"/>
-      <c r="G25" s="30"/>
-      <c r="H25" s="30"/>
-      <c r="I25" s="35" t="s">
+      <c r="A25" s="69"/>
+      <c r="B25" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="C25" s="23" t="s">
+        <v>74</v>
+      </c>
+      <c r="D25" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="E25" s="24"/>
+      <c r="F25" s="23"/>
+      <c r="G25" s="23"/>
+      <c r="H25" s="23"/>
+      <c r="I25" s="24" t="s">
         <v>24</v>
       </c>
       <c r="J25" s="12" t="s">
-        <v>131</v>
-      </c>
-      <c r="K25" s="53"/>
+        <v>118</v>
+      </c>
+      <c r="K25" s="48"/>
     </row>
     <row r="26" spans="1:11" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="68"/>
+      <c r="A26" s="69"/>
       <c r="B26" s="24" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C26" s="23" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D26" s="24" t="s">
         <v>18</v>
@@ -2036,20 +2015,20 @@
         <v>24</v>
       </c>
       <c r="J26" s="12" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="K26" s="48"/>
     </row>
     <row r="27" spans="1:11" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="68"/>
+      <c r="A27" s="69"/>
       <c r="B27" s="24" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C27" s="23" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D27" s="24" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="E27" s="24"/>
       <c r="F27" s="23"/>
@@ -2059,229 +2038,206 @@
         <v>24</v>
       </c>
       <c r="J27" s="12" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="K27" s="48"/>
     </row>
     <row r="28" spans="1:11" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="68"/>
-      <c r="B28" s="24" t="s">
-        <v>71</v>
-      </c>
-      <c r="C28" s="23" t="s">
-        <v>77</v>
-      </c>
-      <c r="D28" s="24" t="s">
+      <c r="A28" s="70"/>
+      <c r="B28" s="36" t="s">
+        <v>78</v>
+      </c>
+      <c r="C28" s="43" t="s">
+        <v>43</v>
+      </c>
+      <c r="D28" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="E28" s="24"/>
-      <c r="F28" s="23"/>
-      <c r="G28" s="23"/>
-      <c r="H28" s="23"/>
-      <c r="I28" s="24" t="s">
+      <c r="E28" s="36"/>
+      <c r="F28" s="43"/>
+      <c r="G28" s="43"/>
+      <c r="H28" s="43"/>
+      <c r="I28" s="36" t="s">
         <v>24</v>
       </c>
       <c r="J28" s="12" t="s">
-        <v>131</v>
-      </c>
-      <c r="K28" s="48"/>
-    </row>
-    <row r="29" spans="1:11" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="69"/>
-      <c r="B29" s="36" t="s">
-        <v>78</v>
-      </c>
-      <c r="C29" s="43" t="s">
-        <v>43</v>
-      </c>
-      <c r="D29" s="36" t="s">
-        <v>30</v>
-      </c>
-      <c r="E29" s="36"/>
-      <c r="F29" s="43"/>
-      <c r="G29" s="43"/>
-      <c r="H29" s="43"/>
-      <c r="I29" s="36" t="s">
+        <v>118</v>
+      </c>
+      <c r="K28" s="54"/>
+    </row>
+    <row r="29" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="57"/>
+      <c r="B29" s="58"/>
+      <c r="C29" s="58"/>
+      <c r="D29" s="58"/>
+      <c r="E29" s="58"/>
+      <c r="F29" s="58"/>
+      <c r="G29" s="58"/>
+      <c r="H29" s="58"/>
+      <c r="I29" s="58"/>
+      <c r="J29" s="58"/>
+      <c r="K29" s="59"/>
+    </row>
+    <row r="30" spans="1:11" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="65" t="s">
+        <v>90</v>
+      </c>
+      <c r="B30" s="46" t="s">
+        <v>80</v>
+      </c>
+      <c r="C30" s="46" t="s">
+        <v>79</v>
+      </c>
+      <c r="D30" s="35" t="s">
+        <v>38</v>
+      </c>
+      <c r="E30" s="35"/>
+      <c r="F30" s="30"/>
+      <c r="G30" s="30"/>
+      <c r="H30" s="30"/>
+      <c r="I30" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="J29" s="12" t="s">
-        <v>131</v>
-      </c>
-      <c r="K29" s="54"/>
-    </row>
-    <row r="30" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="56"/>
-      <c r="B30" s="57"/>
-      <c r="C30" s="57"/>
-      <c r="D30" s="57"/>
-      <c r="E30" s="57"/>
-      <c r="F30" s="57"/>
-      <c r="G30" s="57"/>
-      <c r="H30" s="57"/>
-      <c r="I30" s="57"/>
-      <c r="J30" s="57"/>
-      <c r="K30" s="58"/>
+      <c r="J30" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="K30" s="53"/>
     </row>
     <row r="31" spans="1:11" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="64" t="s">
-        <v>90</v>
-      </c>
-      <c r="B31" s="46" t="s">
-        <v>80</v>
-      </c>
-      <c r="C31" s="46" t="s">
-        <v>79</v>
-      </c>
-      <c r="D31" s="35" t="s">
-        <v>38</v>
-      </c>
-      <c r="E31" s="35"/>
-      <c r="F31" s="30"/>
-      <c r="G31" s="30"/>
-      <c r="H31" s="30"/>
-      <c r="I31" s="35" t="s">
+      <c r="A31" s="66"/>
+      <c r="B31" s="45" t="s">
+        <v>81</v>
+      </c>
+      <c r="C31" s="45" t="s">
+        <v>44</v>
+      </c>
+      <c r="D31" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="E31" s="24"/>
+      <c r="F31" s="23"/>
+      <c r="G31" s="23"/>
+      <c r="H31" s="23"/>
+      <c r="I31" s="24" t="s">
         <v>24</v>
       </c>
       <c r="J31" s="12" t="s">
-        <v>131</v>
-      </c>
-      <c r="K31" s="53"/>
-    </row>
-    <row r="32" spans="1:11" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="65"/>
+        <v>118</v>
+      </c>
+      <c r="K31" s="48"/>
+    </row>
+    <row r="32" spans="1:11" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="66"/>
       <c r="B32" s="45" t="s">
-        <v>81</v>
+        <v>104</v>
       </c>
       <c r="C32" s="45" t="s">
-        <v>44</v>
+        <v>83</v>
       </c>
       <c r="D32" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="E32" s="24"/>
+      <c r="E32" s="56"/>
       <c r="F32" s="23"/>
       <c r="G32" s="23"/>
-      <c r="H32" s="23"/>
+      <c r="H32" s="11" t="s">
+        <v>110</v>
+      </c>
       <c r="I32" s="24" t="s">
         <v>24</v>
       </c>
       <c r="J32" s="12" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="K32" s="48"/>
     </row>
     <row r="33" spans="1:11" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="65"/>
+      <c r="A33" s="66"/>
       <c r="B33" s="45" t="s">
-        <v>110</v>
+        <v>82</v>
       </c>
       <c r="C33" s="45" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D33" s="24" t="s">
-        <v>18</v>
-      </c>
-      <c r="E33" s="73"/>
+        <v>30</v>
+      </c>
+      <c r="E33" s="56"/>
       <c r="F33" s="23"/>
       <c r="G33" s="23"/>
       <c r="H33" s="11" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="I33" s="24" t="s">
         <v>24</v>
       </c>
       <c r="J33" s="12" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="K33" s="48"/>
     </row>
-    <row r="34" spans="1:11" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="65"/>
-      <c r="B34" s="45" t="s">
-        <v>82</v>
-      </c>
-      <c r="C34" s="45" t="s">
-        <v>84</v>
+    <row r="34" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A34" s="66"/>
+      <c r="B34" s="47" t="s">
+        <v>105</v>
+      </c>
+      <c r="C34" s="21" t="s">
+        <v>45</v>
       </c>
       <c r="D34" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="E34" s="73"/>
+      <c r="E34" s="24"/>
       <c r="F34" s="23"/>
       <c r="G34" s="23"/>
-      <c r="H34" s="11" t="s">
-        <v>119</v>
-      </c>
+      <c r="H34" s="23"/>
       <c r="I34" s="24" t="s">
         <v>24</v>
       </c>
       <c r="J34" s="12" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="K34" s="48"/>
     </row>
-    <row r="35" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A35" s="65"/>
-      <c r="B35" s="47" t="s">
-        <v>111</v>
-      </c>
-      <c r="C35" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="D35" s="24" t="s">
-        <v>30</v>
-      </c>
-      <c r="E35" s="24"/>
-      <c r="F35" s="23"/>
-      <c r="G35" s="23"/>
-      <c r="H35" s="23"/>
-      <c r="I35" s="24" t="s">
-        <v>24</v>
-      </c>
-      <c r="J35" s="12" t="s">
-        <v>131</v>
-      </c>
-      <c r="K35" s="48"/>
+    <row r="35" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="67"/>
+      <c r="B35" s="36"/>
+      <c r="C35" s="43"/>
+      <c r="D35" s="36"/>
+      <c r="E35" s="36"/>
+      <c r="F35" s="43"/>
+      <c r="G35" s="43"/>
+      <c r="H35" s="43"/>
+      <c r="I35" s="43"/>
+      <c r="J35" s="43"/>
+      <c r="K35" s="54"/>
     </row>
     <row r="36" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="66"/>
-      <c r="B36" s="36"/>
-      <c r="C36" s="43"/>
-      <c r="D36" s="36"/>
-      <c r="E36" s="36"/>
-      <c r="F36" s="43"/>
-      <c r="G36" s="43"/>
-      <c r="H36" s="43"/>
-      <c r="I36" s="43"/>
-      <c r="J36" s="43"/>
-      <c r="K36" s="54"/>
-    </row>
-    <row r="37" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="56"/>
-      <c r="B37" s="57"/>
-      <c r="C37" s="57"/>
-      <c r="D37" s="57"/>
-      <c r="E37" s="57"/>
-      <c r="F37" s="57"/>
-      <c r="G37" s="57"/>
-      <c r="H37" s="57"/>
-      <c r="I37" s="57"/>
-      <c r="J37" s="57"/>
-      <c r="K37" s="58"/>
+      <c r="A36" s="57"/>
+      <c r="B36" s="58"/>
+      <c r="C36" s="58"/>
+      <c r="D36" s="58"/>
+      <c r="E36" s="58"/>
+      <c r="F36" s="58"/>
+      <c r="G36" s="58"/>
+      <c r="H36" s="58"/>
+      <c r="I36" s="58"/>
+      <c r="J36" s="58"/>
+      <c r="K36" s="59"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A37:K37"/>
+    <mergeCell ref="A36:K36"/>
     <mergeCell ref="A5:A6"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="A12:A17"/>
-    <mergeCell ref="A19:A23"/>
-    <mergeCell ref="A25:A29"/>
-    <mergeCell ref="A31:A36"/>
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="A13:A17"/>
+    <mergeCell ref="A19:A22"/>
+    <mergeCell ref="A24:A28"/>
+    <mergeCell ref="A30:A35"/>
     <mergeCell ref="A18:K18"/>
-    <mergeCell ref="A11:K11"/>
-    <mergeCell ref="A24:K24"/>
-    <mergeCell ref="A30:K30"/>
+    <mergeCell ref="A12:K12"/>
+    <mergeCell ref="A23:K23"/>
+    <mergeCell ref="A29:K29"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="7.874015748031496E-2" right="7.874015748031496E-2" top="0.74803149606299213" bottom="0.19685039370078741" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>